<commit_message>
Removed allure report result files which are redundant on GitHub
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/comprehensive_testdata.xlsx
+++ b/src/test/resources/testdata/comprehensive_testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2421386\Salenium\BookMyShow\bookmyshow-1\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31ACA270-8615-40BB-A132-F52BB87C7BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34167F0-CD2D-4FF4-9FB1-51930B19323C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchData" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,13 @@
     <sheet name="EventsTestData" sheetId="4" r:id="rId4"/>
     <sheet name="TestScenarios" sheetId="5" r:id="rId5"/>
     <sheet name="ExpectedResults" sheetId="6" r:id="rId6"/>
-    <sheet name="TestConfiguration" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="250">
   <si>
     <t>City</t>
   </si>
@@ -799,126 +798,6 @@
   </si>
   <si>
     <t>User-friendly message displayed</t>
-  </si>
-  <si>
-    <t>Configuration_Key</t>
-  </si>
-  <si>
-    <t>Configuration_Value</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Browser</t>
-  </si>
-  <si>
-    <t>chrome</t>
-  </si>
-  <si>
-    <t>Browser for test execution</t>
-  </si>
-  <si>
-    <t>Base_URL</t>
-  </si>
-  <si>
-    <t>https://in.bookmyshow.com</t>
-  </si>
-  <si>
-    <t>BookMyShow application URL</t>
-  </si>
-  <si>
-    <t>Implicit_Wait</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Implicit wait timeout in seconds</t>
-  </si>
-  <si>
-    <t>Explicit_Wait</t>
-  </si>
-  <si>
-    <t>Explicit wait timeout in seconds</t>
-  </si>
-  <si>
-    <t>Page_Load_Timeout</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>Page load timeout in seconds</t>
-  </si>
-  <si>
-    <t>Test_Data_File</t>
-  </si>
-  <si>
-    <t>testdata.xlsx</t>
-  </si>
-  <si>
-    <t>Test data Excel file name</t>
-  </si>
-  <si>
-    <t>Screenshot_Path</t>
-  </si>
-  <si>
-    <t>test-output/screenshots/</t>
-  </si>
-  <si>
-    <t>Screenshot storage path</t>
-  </si>
-  <si>
-    <t>Report_Path</t>
-  </si>
-  <si>
-    <t>test-output/ExtentReports/</t>
-  </si>
-  <si>
-    <t>Test report storage path</t>
-  </si>
-  <si>
-    <t>Default_City</t>
-  </si>
-  <si>
-    <t>Default city for testing</t>
-  </si>
-  <si>
-    <t>Test_Environment</t>
-  </si>
-  <si>
-    <t>Production</t>
-  </si>
-  <si>
-    <t>Testing environment</t>
-  </si>
-  <si>
-    <t>Parallel_Execution</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>Enable parallel test execution</t>
-  </si>
-  <si>
-    <t>Retry_Count</t>
-  </si>
-  <si>
-    <t>Number of retries for failed tests</t>
-  </si>
-  <si>
-    <t>Video_Recording</t>
-  </si>
-  <si>
-    <t>Enable video recording</t>
-  </si>
-  <si>
-    <t>Headless_Mode</t>
-  </si>
-  <si>
-    <t>Run browser in headless mode</t>
   </si>
 </sst>
 </file>
@@ -1936,7 +1815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2211,8 +2090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2488,7 +2367,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2689,187 +2570,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:C15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="36" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>253</v>
-      </c>
-      <c r="B2" t="s">
-        <v>254</v>
-      </c>
-      <c r="C2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>256</v>
-      </c>
-      <c r="B3" t="s">
-        <v>257</v>
-      </c>
-      <c r="C3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>259</v>
-      </c>
-      <c r="B4" t="s">
-        <v>260</v>
-      </c>
-      <c r="C4" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>262</v>
-      </c>
-      <c r="B5" t="s">
-        <v>260</v>
-      </c>
-      <c r="C5" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>264</v>
-      </c>
-      <c r="B6" t="s">
-        <v>265</v>
-      </c>
-      <c r="C6" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>267</v>
-      </c>
-      <c r="B7" t="s">
-        <v>268</v>
-      </c>
-      <c r="C7" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>270</v>
-      </c>
-      <c r="B8" t="s">
-        <v>271</v>
-      </c>
-      <c r="C8" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>273</v>
-      </c>
-      <c r="B9" t="s">
-        <v>274</v>
-      </c>
-      <c r="C9" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>276</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>278</v>
-      </c>
-      <c r="B11" t="s">
-        <v>279</v>
-      </c>
-      <c r="C11" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>281</v>
-      </c>
-      <c r="B12" t="s">
-        <v>282</v>
-      </c>
-      <c r="C12" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>284</v>
-      </c>
-      <c r="B13" t="s">
-        <v>163</v>
-      </c>
-      <c r="C13" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>286</v>
-      </c>
-      <c r="B14" t="s">
-        <v>282</v>
-      </c>
-      <c r="C14" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>288</v>
-      </c>
-      <c r="B15" t="s">
-        <v>282</v>
-      </c>
-      <c r="C15" t="s">
-        <v>289</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>